<commit_message>
Read capacity parameters. Use timestamp to retrive only valid data.
</commit_message>
<xml_diff>
--- a/schedule_days.xlsx
+++ b/schedule_days.xlsx
@@ -434,165 +434,101 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>02.09.2022</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>05.09.2022</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>06.09.2022</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>07.09.2022</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>08.09.2022</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>09.09.2022</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>12.09.2022</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>13.09.2022</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>14.09.2022</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>15.09.2022</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>16.09.2022</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>19.09.2022</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>20.09.2022</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>21.09.2022</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>22.09.2022</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>23.09.2022</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>26.09.2022</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>27.09.2022</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>28.09.2022</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>29.09.2022</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>30.09.2022</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>03.10.2022</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>04.10.2022</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>05.10.2022</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>06.10.2022</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>07.10.2022</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>10.10.2022</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>11.10.2022</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>12.10.2022</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>13.10.2022</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>14.10.2022</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>17.10.2022</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="2">

</xml_diff>